<commit_message>
update on HDMI to MIPI
</commit_message>
<xml_diff>
--- a/bom/hdmi_to_mipi-dsi_converter version 2.xlsx
+++ b/bom/hdmi_to_mipi-dsi_converter version 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\KICAD DESIGNS\KICAD CLONES IN USE\hdmi_to_mipi-dsi_converter\hdmi_to_mipi-dsi_converter\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B874A9-5909-4B28-86A3-FA42062EC463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA137A5-0152-42EF-BA34-34DF4118CD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hdmi_to_mipi-dsi_converter" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="172">
   <si>
     <t>REFERNCE</t>
   </si>
@@ -46,9 +46,6 @@
     <t>QUANTITY</t>
   </si>
   <si>
-    <t>&gt;  C1, C3, C5, C7, C9, C11, C13, C14, C48, C50, C52, C54, C56, C58, C60, C61</t>
-  </si>
-  <si>
     <t>10n</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>LCSC</t>
   </si>
   <si>
-    <t>&gt;  C16, C22</t>
-  </si>
-  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -76,30 +70,12 @@
     <t>CC0603KRX5R6BB106</t>
   </si>
   <si>
-    <t xml:space="preserve">    C17</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
     <t>CC0603KRX5R8BB105</t>
   </si>
   <si>
-    <t>&gt;  C19, C20</t>
-  </si>
-  <si>
-    <t>Resistor_SMD:R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>Murata Electronics</t>
-  </si>
-  <si>
-    <t>GRM21BR61E106KA73L</t>
-  </si>
-  <si>
-    <t>&gt;  C2, C4, C6, C8, C10, C12, C23, C25, C29, C30, C33-C35, C37-C39, C42, C43, C49, C51, C53, C55, C57, C59, C62, C64-C66</t>
-  </si>
-  <si>
     <t>0.1u</t>
   </si>
   <si>
@@ -109,9 +85,6 @@
     <t>CC0402KRX7R7BB104</t>
   </si>
   <si>
-    <t>&gt;  C26, C63</t>
-  </si>
-  <si>
     <t>0.01u</t>
   </si>
   <si>
@@ -139,18 +112,6 @@
     <t>DigiKey</t>
   </si>
   <si>
-    <t xml:space="preserve">    C32</t>
-  </si>
-  <si>
-    <t>1.5nF</t>
-  </si>
-  <si>
-    <t>C0805C152KDRACAUTO</t>
-  </si>
-  <si>
-    <t>&gt;  C15, C18, C21, C24, C36</t>
-  </si>
-  <si>
     <t>10u</t>
   </si>
   <si>
@@ -178,42 +139,6 @@
     <t>4.7u</t>
   </si>
   <si>
-    <t xml:space="preserve">    C67</t>
-  </si>
-  <si>
-    <t>8.2nF</t>
-  </si>
-  <si>
-    <t>Capacitor_SMD:C_1206_3216Metric</t>
-  </si>
-  <si>
-    <t>C1206C822KDRACAUTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    C68</t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>Capacitor_SMD:C_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>CL21B104KCFWPJE</t>
-  </si>
-  <si>
-    <t>&gt;  C69-C71</t>
-  </si>
-  <si>
-    <t>22uF</t>
-  </si>
-  <si>
-    <t>Resistor_SMD:R_0201_0603Metric</t>
-  </si>
-  <si>
-    <t>GRM188R60J226MEA0D</t>
-  </si>
-  <si>
     <t>&gt;  C72, C73</t>
   </si>
   <si>
@@ -256,18 +181,12 @@
     <t xml:space="preserve">    FB2</t>
   </si>
   <si>
-    <t xml:space="preserve">    FB3</t>
-  </si>
-  <si>
     <t>FBMJ1608HS280NTR</t>
   </si>
   <si>
     <t>Resistor_SMD:R_0603_1608Metric</t>
   </si>
   <si>
-    <t>&gt;  J1, J2</t>
-  </si>
-  <si>
     <t>HDMI-019S</t>
   </si>
   <si>
@@ -310,15 +229,6 @@
     <t>TerminalBlock_4Ucon:TerminalBlock_4Ucon_1x02_P3.50mm_Horizontal</t>
   </si>
   <si>
-    <t xml:space="preserve">    L1</t>
-  </si>
-  <si>
-    <t>74438357068_ind:74438357068</t>
-  </si>
-  <si>
-    <t>6.8uH_7mOHM</t>
-  </si>
-  <si>
     <t>&gt;  R1, R15</t>
   </si>
   <si>
@@ -355,24 +265,15 @@
     <t xml:space="preserve">    R9</t>
   </si>
   <si>
-    <t>&gt;  R6, R7, R10, R11, R20-R22</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
     <t xml:space="preserve">    R12</t>
   </si>
   <si>
-    <t>&gt;  R13, R14</t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
-    <t>&gt;  R23, R24, R29, R30</t>
-  </si>
-  <si>
     <t>2.2K</t>
   </si>
   <si>
@@ -385,33 +286,6 @@
     <t>RMCF0603FT61K9</t>
   </si>
   <si>
-    <t xml:space="preserve">    R26</t>
-  </si>
-  <si>
-    <t>10.2k</t>
-  </si>
-  <si>
-    <t>CRCW060310K2FKEAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    R27</t>
-  </si>
-  <si>
-    <t>1.96k</t>
-  </si>
-  <si>
-    <t>RMCF0603FT1K96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    R28</t>
-  </si>
-  <si>
-    <t>0R</t>
-  </si>
-  <si>
-    <t>&gt;  R32, R34</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
@@ -454,9 +328,6 @@
     <t>ME6211A33PG-N</t>
   </si>
   <si>
-    <t>&gt;  U4, U9</t>
-  </si>
-  <si>
     <t>TC358870XBG_NOK_</t>
   </si>
   <si>
@@ -475,18 +346,6 @@
     <t>MCP1700-3302E_SOT23</t>
   </si>
   <si>
-    <t xml:space="preserve">    U6</t>
-  </si>
-  <si>
-    <t>TPS54332DDA</t>
-  </si>
-  <si>
-    <t>TPS54332:NOPB</t>
-  </si>
-  <si>
-    <t>TPS54332DDAR</t>
-  </si>
-  <si>
     <t xml:space="preserve">    U7</t>
   </si>
   <si>
@@ -505,9 +364,6 @@
     <t>Barrel - Audio Connectors:QFN40P180X180X55-12N</t>
   </si>
   <si>
-    <t>&gt;  Y1, Y3</t>
-  </si>
-  <si>
     <t>CRYSTAL_48MHZ</t>
   </si>
   <si>
@@ -562,9 +418,6 @@
     <t>RC0402JR-072KL</t>
   </si>
   <si>
-    <t>würth Elektronik</t>
-  </si>
-  <si>
     <t>RC0402FR-0747KL</t>
   </si>
   <si>
@@ -592,15 +445,9 @@
     <t>RC0402JR-072K2L</t>
   </si>
   <si>
-    <t>RC0603JR-070RL</t>
-  </si>
-  <si>
     <t>Stackpole Electronics Inc</t>
   </si>
   <si>
-    <t>Vishay Dale</t>
-  </si>
-  <si>
     <t>Microchip Tech</t>
   </si>
   <si>
@@ -613,12 +460,6 @@
     <t>MCP1700T-3302E/TT</t>
   </si>
   <si>
-    <t>Texas instruments</t>
-  </si>
-  <si>
-    <t>DigiPart</t>
-  </si>
-  <si>
     <t>STMicroelectronics</t>
   </si>
   <si>
@@ -637,12 +478,6 @@
     <t>7325-0800A2010-00</t>
   </si>
   <si>
-    <t>KEMET</t>
-  </si>
-  <si>
-    <t>Samsung Electro-Mechanics</t>
-  </si>
-  <si>
     <t>LITEON</t>
   </si>
   <si>
@@ -659,6 +494,48 @@
   </si>
   <si>
     <t xml:space="preserve">Axelite Tech </t>
+  </si>
+  <si>
+    <t>C1, C3, C5, C7, C9, C11, C13, C14, C48, C50, C52, C54, C56, C58, C60, C61</t>
+  </si>
+  <si>
+    <t>C17, C20</t>
+  </si>
+  <si>
+    <t>C16, C22</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C2, C4, C6, C8, C10, C12, C23, C25, C29, C30, C33-C35, C37-C39, C42, C43, C49, C51, C53, C55, C57, C59, C62, C64-C66</t>
+  </si>
+  <si>
+    <t>C26, C63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    FB3, FB5</t>
+  </si>
+  <si>
+    <t>C15, C18, C19, C21, C24, C36</t>
+  </si>
+  <si>
+    <t>J1, J2</t>
+  </si>
+  <si>
+    <t>R6, R7, R10, R11, R20-R22</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> R13, R14</t>
+  </si>
+  <si>
+    <t>R23, R24, R29, R30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> R32, R34</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> U4, U9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Y1, Y3</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1048,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
@@ -1186,9 +1063,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1546,10 +1420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1558,7 +1432,7 @@
     <col min="2" max="2" width="17.88671875" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
     <col min="4" max="4" width="15.21875" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" customWidth="1"/>
   </cols>
@@ -1595,13 +1469,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4">
@@ -1609,13 +1483,13 @@
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" s="4">
         <v>16</v>
@@ -1623,13 +1497,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4">
@@ -1637,13 +1511,13 @@
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" s="4">
         <v>2</v>
@@ -1651,13 +1525,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>18</v>
+        <v>159</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4">
@@ -1665,119 +1539,119 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>161</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" s="4">
-        <v>2</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>25</v>
+        <v>162</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="I6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J6" s="4">
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J7" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J8" s="4">
         <v>1</v>
@@ -1785,25 +1659,23 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="J9" s="4">
         <v>1</v>
@@ -1811,101 +1683,105 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>164</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="H10" s="4" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="J10" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="H11" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="J11" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J12" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J13" s="4">
         <v>2</v>
@@ -1913,25 +1789,25 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>49</v>
+      <c r="G14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J14" s="4">
         <v>2</v>
@@ -1939,25 +1815,25 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>168</v>
+      <c r="G15" t="s">
+        <v>152</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="J15" s="4">
         <v>2</v>
@@ -1965,25 +1841,27 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" t="s">
-        <v>205</v>
+      <c r="F16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J16" s="4">
         <v>1</v>
@@ -1991,25 +1869,25 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" t="s">
-        <v>206</v>
+      <c r="G17" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J17" s="4">
         <v>1</v>
@@ -2017,77 +1895,77 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>62</v>
+        <v>156</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" t="s">
-        <v>23</v>
+      <c r="G18" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J18" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>10</v>
+        <v>156</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>169</v>
+      <c r="G19" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="J19" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>66</v>
+        <v>163</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>68</v>
+        <v>156</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" t="s">
-        <v>207</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>170</v>
+      <c r="G20" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J20" s="4">
         <v>2</v>
@@ -2095,53 +1973,51 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>69</v>
+        <v>165</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>208</v>
+      <c r="F21" s="4"/>
+      <c r="G21" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>38</v>
+        <v>55</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="J21" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>74</v>
+      <c r="G22" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J22" s="4">
         <v>1</v>
@@ -2149,77 +2025,77 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>211</v>
+        <v>62</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>79</v>
+      <c r="G23" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H23" s="6">
+        <v>1050170001</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="J23" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>211</v>
+        <v>65</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>79</v>
+      <c r="G24" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="J24" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>211</v>
+        <v>68</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>79</v>
+      <c r="G25" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="J25" s="4">
         <v>1</v>
@@ -2227,25 +2103,25 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="6" t="s">
-        <v>171</v>
+      <c r="G26" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>13</v>
+        <v>131</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="J26" s="4">
         <v>2</v>
@@ -2253,77 +2129,77 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>173</v>
+      <c r="G27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J27" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="H28" s="6">
-        <v>1050170001</v>
+      <c r="G28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J28" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>176</v>
+      <c r="G29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J29" s="4">
         <v>2</v>
@@ -2331,25 +2207,25 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>178</v>
+      <c r="G30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J30" s="4">
         <v>1</v>
@@ -2357,27 +2233,25 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" s="4">
-        <v>74438357068</v>
+        <v>80</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="D31" s="4"/>
-      <c r="E31" s="4" t="s">
-        <v>98</v>
-      </c>
+      <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="H31" s="4">
-        <v>74438357068</v>
+      <c r="G31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="J31" s="4">
         <v>1</v>
@@ -2385,129 +2259,129 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>99</v>
+        <v>166</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>179</v>
+        <v>10</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J32" s="4">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>181</v>
+        <v>10</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="J33" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>104</v>
+        <v>167</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>182</v>
+        <v>10</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J34" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>106</v>
+        <v>168</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>183</v>
+        <v>140</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="J35" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>184</v>
+        <v>141</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="J36" s="4">
         <v>1</v>
@@ -2515,77 +2389,77 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>110</v>
+        <v>169</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>185</v>
+        <v>137</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="J37" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>186</v>
+        <v>10</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="J38" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="4" t="s">
-        <v>11</v>
+      <c r="G39" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>187</v>
+        <v>92</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J39" s="4">
         <v>1</v>
@@ -2593,103 +2467,107 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="E40" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>188</v>
+        <v>157</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J40" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4" t="s">
-        <v>11</v>
+        <v>143</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>189</v>
+        <v>101</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="J41" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4" t="s">
-        <v>191</v>
+        <v>105</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>38</v>
+        <v>104</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="J42" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>123</v>
+      <c r="G43" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="J43" s="4">
         <v>1</v>
@@ -2697,25 +2575,25 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="4" t="s">
-        <v>191</v>
+      <c r="G44" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="J44" s="4">
         <v>1</v>
@@ -2723,25 +2601,25 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="4" t="s">
-        <v>11</v>
+      <c r="G45" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>190</v>
+        <v>112</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="J45" s="4">
         <v>1</v>
@@ -2749,25 +2627,25 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>129</v>
+        <v>171</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>38</v>
+      <c r="G46" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="J46" s="4">
         <v>2</v>
@@ -2775,299 +2653,35 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>181</v>
+      <c r="G47" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="J47" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J48" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="I49" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J49" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J50" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="J51" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="H52" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J52" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="J53" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="I54" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J54" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J55" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="I56" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="J56" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J57" s="4">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H19" r:id="rId1" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_YAGEO-CC0402KRX7R9BB103_C60133.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H20" r:id="rId2" display="https://www.digikey.com/en/products/detail/lite-on-inc/LTST-C191KRKT/386837" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G19" r:id="rId3" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_YAGEO-CC0402KRX7R9BB103_C60133.html" xr:uid="{83FCF2A8-35F7-4F62-8D4D-089858EB5642}"/>
+    <hyperlink ref="H14" r:id="rId1" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_YAGEO-CC0402KRX7R9BB103_C60133.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H15" r:id="rId2" display="https://www.digikey.com/en/products/detail/lite-on-inc/LTST-C191KRKT/386837" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G14" r:id="rId3" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_YAGEO-CC0402KRX7R9BB103_C60133.html" xr:uid="{83FCF2A8-35F7-4F62-8D4D-089858EB5642}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>